<commit_message>
modified the format to fit the event table
</commit_message>
<xml_diff>
--- a/kronos/exceldata.xlsx
+++ b/kronos/exceldata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12900" yWindow="1580" windowWidth="14320" windowHeight="9920" tabRatio="500"/>
+    <workbookView xWindow="1420" yWindow="1740" windowWidth="14320" windowHeight="9920" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,10 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
-  <si>
-    <t>Summary</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>dtstart</t>
   </si>
@@ -41,9 +38,6 @@
     <t>private</t>
   </si>
   <si>
-    <t>t</t>
-  </si>
-  <si>
     <t>userid</t>
   </si>
   <si>
@@ -51,6 +45,9 @@
   </si>
   <si>
     <t>event2</t>
+  </si>
+  <si>
+    <t>summary</t>
   </si>
 </sst>
 </file>
@@ -369,7 +366,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -380,24 +377,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1">
         <v>42493.416666666664</v>
@@ -405,8 +402,8 @@
       <c r="C2" s="1">
         <v>42493.5</v>
       </c>
-      <c r="D2" t="s">
-        <v>4</v>
+      <c r="D2" t="b">
+        <v>1</v>
       </c>
       <c r="E2">
         <v>18</v>
@@ -414,7 +411,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1">
         <v>42494.416666666664</v>
@@ -422,8 +419,8 @@
       <c r="C3" s="1">
         <v>42494.458333333336</v>
       </c>
-      <c r="D3" t="s">
-        <v>4</v>
+      <c r="D3" t="b">
+        <v>0</v>
       </c>
       <c r="E3">
         <v>18</v>

</xml_diff>